<commit_message>
Code refactoring and added test cases
</commit_message>
<xml_diff>
--- a/Processes/DocumentProcessing/output/Tiefland%20Glass%20AG%20Inv850888.xlsx
+++ b/Processes/DocumentProcessing/output/Tiefland%20Glass%20AG%20Inv850888.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <x:si>
     <x:t>Invoice No.</x:t>
   </x:si>
@@ -92,7 +92,7 @@
     <x:t>Werneckstrasse 231 80802 Munich Germany</x:t>
   </x:si>
   <x:si>
-    <x:t>EUR</x:t>
+    <x:t>USD</x:t>
   </x:si>
   <x:si>
     <x:t>30964.00</x:t>
@@ -159,10 +159,16 @@
     <x:t>4</x:t>
   </x:si>
   <x:si>
+    <x:t>7741</x:t>
+  </x:si>
+  <x:si>
     <x:t>30964</x:t>
   </x:si>
   <x:si>
     <x:t>4.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7741.00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -197,8 +203,44 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="66">
+  <x:cellStyleXfs count="78">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -975,8 +1017,11 @@
       <x:c r="C2" s="2" t="s">
         <x:v>40</x:v>
       </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
       <x:c r="E2" s="2" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1024,7 +1069,10 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E2" s="2" t="s">
         <x:v>23</x:v>

</xml_diff>

<commit_message>
Updated SAP Server. Code refactoring and added test cases.
</commit_message>
<xml_diff>
--- a/Processes/DocumentProcessing/output/Tiefland%20Glass%20AG%20Inv850888.xlsx
+++ b/Processes/DocumentProcessing/output/Tiefland%20Glass%20AG%20Inv850888.xlsx
@@ -92,7 +92,7 @@
     <x:t>Werneckstrasse 231 80802 Munich Germany</x:t>
   </x:si>
   <x:si>
-    <x:t>USD</x:t>
+    <x:t>EUR</x:t>
   </x:si>
   <x:si>
     <x:t>30964.00</x:t>
@@ -104,7 +104,7 @@
     <x:t>34060.4</x:t>
   </x:si>
   <x:si>
-    <x:t>due in 45 days</x:t>
+    <x:t>45 days</x:t>
   </x:si>
   <x:si>
     <x:t>2020-05-22</x:t>
@@ -203,8 +203,44 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="78">
+  <x:cellStyleXfs count="90">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>